<commit_message>
modify model from table_view modify article sync
</commit_message>
<xml_diff>
--- a/modules/kckr/assets/template/import_karya_template.xlsx
+++ b/modules/kckr/assets/template/import_karya_template.xlsx
@@ -14,10 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>CATEGORY</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="58">
   <si>
     <t>TITLE</t>
   </si>
@@ -32,14 +29,181 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Tungau (Akarina) dan Pengolahannya</t>
+  </si>
+  <si>
+    <t>Moch.Sodiq</t>
+  </si>
+  <si>
+    <t>Slamet Abadi</t>
+  </si>
+  <si>
+    <t>Mekanika Kekuatan Material Edisi 2</t>
+  </si>
+  <si>
+    <t>Ramses Yohannes Hutaean</t>
+  </si>
+  <si>
+    <t>Akuntansi Pemerintah Berbasis Akrual</t>
+  </si>
+  <si>
+    <t>Soeradi</t>
+  </si>
+  <si>
+    <t>Repong Damar</t>
+  </si>
+  <si>
+    <t>Sugeng P.Harianto</t>
+  </si>
+  <si>
+    <t>Struktur dan Ikatan Kimia</t>
+  </si>
+  <si>
+    <t>Saludin Muis</t>
+  </si>
+  <si>
+    <t>Sistem dan teknologi informasi</t>
+  </si>
+  <si>
+    <t>Richardus Eko Indrajit</t>
+  </si>
+  <si>
+    <t>Potensi populasi empat rumpun kambing di Provinsi Lampung</t>
+  </si>
+  <si>
+    <t>Sulastri</t>
+  </si>
+  <si>
+    <t>Pragmatik edisi 2</t>
+  </si>
+  <si>
+    <t>Jumanto</t>
+  </si>
+  <si>
+    <t>Antropologi Wayang</t>
+  </si>
+  <si>
+    <t>Suwardi Endraswara</t>
+  </si>
+  <si>
+    <t>Noun Phrases second edition</t>
+  </si>
+  <si>
+    <t>Memahami kontrsepsi hormonal wanita</t>
+  </si>
+  <si>
+    <t>Sri Warsih</t>
+  </si>
+  <si>
+    <t>Konsep blue economy</t>
+  </si>
+  <si>
+    <t>Ali Musa Pasaribu</t>
+  </si>
+  <si>
+    <t>Filsafat Pendidikan</t>
+  </si>
+  <si>
+    <t>Septian Aji Permana</t>
+  </si>
+  <si>
+    <t>Persuasi Komunikasi dan Kebijakan publik</t>
+  </si>
+  <si>
+    <t>Inadia Aristyavani</t>
+  </si>
+  <si>
+    <t>Politik Identitas di Indonesia</t>
+  </si>
+  <si>
+    <t>Agus Hiplunudin</t>
+  </si>
+  <si>
+    <t>Sejarah Nasional Indonesia</t>
+  </si>
+  <si>
+    <t>Iskandar Syah</t>
+  </si>
+  <si>
+    <t>Penguat operasional (Op-Amp) Teori Lanjutan dan Pemakaian</t>
+  </si>
+  <si>
+    <t>Penguat operasional (Op-Amp) Teori dan Rangkaian Dasar</t>
+  </si>
+  <si>
+    <t>Metodologi Penelitian Ekonomi dan Bisnis edisi 2</t>
+  </si>
+  <si>
+    <t>Konsep ekologi dalam Pembangunan Berkelanjutan</t>
+  </si>
+  <si>
+    <t>Astri Rinanti</t>
+  </si>
+  <si>
+    <t>Mekanika Kekuatan Material Tingkat Lanjut Edisi 2</t>
+  </si>
+  <si>
+    <t>Statistika Penelitian Plus Tutorial SPSS</t>
+  </si>
+  <si>
+    <t>Sejuta Manfaat Ikan Lele</t>
+  </si>
+  <si>
+    <t>Revolusi</t>
+  </si>
+  <si>
+    <t>Nyoman Wijana</t>
+  </si>
+  <si>
+    <t>Fenomena Superkonduktor latar belakang dan Landasan Teori</t>
+  </si>
+  <si>
+    <t>Teori Adhesi dan bahan Adhesif</t>
+  </si>
+  <si>
+    <t>Lumpur Pemboran</t>
+  </si>
+  <si>
+    <t>Aris Buntoro</t>
+  </si>
+  <si>
+    <t>Strategi Pembelajaran IPS Kontemporer</t>
+  </si>
+  <si>
+    <t>Perencanaan dan Pengembangan Kurikulum</t>
+  </si>
+  <si>
+    <t>Pengelolaan Limbah edisi 2</t>
+  </si>
+  <si>
+    <t>Arif Zulkifli</t>
+  </si>
+  <si>
+    <t>Aljabar Liner, Matriks dan Vektor</t>
+  </si>
+  <si>
+    <t>CATEGORY CODE</t>
+  </si>
+  <si>
+    <t>mono</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -67,8 +231,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -373,35 +538,551 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
+      </c>
+      <c r="D2">
+        <v>2016</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3">
+        <v>2016</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>2016</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>2016</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6">
+        <v>2016</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7">
+        <v>2016</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8">
+        <v>2016</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9">
+        <v>2016</v>
+      </c>
+      <c r="E9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10">
+        <v>2016</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11">
+        <v>2016</v>
+      </c>
+      <c r="E11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12">
+        <v>2016</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13">
+        <v>2016</v>
+      </c>
+      <c r="E13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14">
+        <v>2016</v>
+      </c>
+      <c r="E14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15">
+        <v>2016</v>
+      </c>
+      <c r="E15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16">
+        <v>2016</v>
+      </c>
+      <c r="E16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17">
+        <v>2016</v>
+      </c>
+      <c r="E17" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18">
+        <v>2016</v>
+      </c>
+      <c r="E18" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19">
+        <v>2016</v>
+      </c>
+      <c r="E19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20">
+        <v>2016</v>
+      </c>
+      <c r="E20" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21">
+        <v>2016</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22">
+        <v>2016</v>
+      </c>
+      <c r="E22" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23">
+        <v>2016</v>
+      </c>
+      <c r="E23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24">
+        <v>2016</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25">
+        <v>2016</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26">
+        <v>2016</v>
+      </c>
+      <c r="E26" t="s">
+        <v>46</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" t="s">
+        <v>47</v>
+      </c>
+      <c r="D27">
+        <v>2016</v>
+      </c>
+      <c r="E27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28">
+        <v>2016</v>
+      </c>
+      <c r="E28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" t="s">
+        <v>49</v>
+      </c>
+      <c r="D29">
+        <v>2016</v>
+      </c>
+      <c r="E29" t="s">
+        <v>50</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30">
+        <v>2016</v>
+      </c>
+      <c r="E30" t="s">
+        <v>30</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31">
+        <v>2016</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32" t="s">
+        <v>53</v>
+      </c>
+      <c r="D32">
+        <v>2016</v>
+      </c>
+      <c r="E32" t="s">
+        <v>54</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>